<commit_message>
Implement ExcelAdapter and Neo4jAdapter
</commit_message>
<xml_diff>
--- a/tests/Fixtures/Excel/books.xlsx
+++ b/tests/Fixtures/Excel/books.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="115">
   <si>
     <t>title</t>
   </si>
@@ -19,13 +19,343 @@
     <t>author</t>
   </si>
   <si>
-    <t>War and Peace</t>
-  </si>
-  <si>
-    <t>Tolstoy, Leo</t>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>publishing year</t>
+  </si>
+  <si>
+    <t>The Hobbit</t>
+  </si>
+  <si>
+    <t>Joyce, James</t>
+  </si>
+  <si>
+    <t>978-1151-5715-0171-9</t>
+  </si>
+  <si>
+    <t>The Sound and the Fury</t>
+  </si>
+  <si>
+    <t>Homer</t>
+  </si>
+  <si>
+    <t>978-7627-1324-7204-3</t>
+  </si>
+  <si>
+    <t>The Adventures of Huckleberry Finn</t>
+  </si>
+  <si>
+    <t>Steinbeck, John</t>
+  </si>
+  <si>
+    <t>978-7716-4343-5217-2</t>
+  </si>
+  <si>
+    <t>The Catcher in the Rye</t>
+  </si>
+  <si>
+    <t>978-3977-8614-5155-4</t>
+  </si>
+  <si>
+    <t>Frankenstein</t>
+  </si>
+  <si>
+    <t>Faulkner, William</t>
+  </si>
+  <si>
+    <t>978-6725-0096-7934-8</t>
+  </si>
+  <si>
+    <t>The Odyssey</t>
+  </si>
+  <si>
+    <t>Salinger, J.D.</t>
+  </si>
+  <si>
+    <t>978-4807-6807-9795-5</t>
+  </si>
+  <si>
+    <t>Hemingway, Ernest</t>
+  </si>
+  <si>
+    <t>978-1640-1391-6321-4</t>
+  </si>
+  <si>
+    <t>The Sun Also Rises</t>
+  </si>
+  <si>
+    <t>Cervantes, Miguel de</t>
+  </si>
+  <si>
+    <t>978-9674-2588-1477-6</t>
+  </si>
+  <si>
+    <t>Flaubert, Gustave</t>
+  </si>
+  <si>
+    <t>978-0078-9884-6018-1</t>
+  </si>
+  <si>
+    <t>The Trial</t>
+  </si>
+  <si>
+    <t>Lee, Harper</t>
+  </si>
+  <si>
+    <t>978-6534-3378-2938-6</t>
+  </si>
+  <si>
+    <t>Jane Eyre</t>
+  </si>
+  <si>
+    <t>Wilde, Oscar</t>
+  </si>
+  <si>
+    <t>978-2744-3619-2362-5</t>
+  </si>
+  <si>
+    <t>The Magic Mountain</t>
+  </si>
+  <si>
+    <t>978-8554-5786-2059-0</t>
+  </si>
+  <si>
+    <t>978-1535-0969-5321-5</t>
+  </si>
+  <si>
+    <t>Oliver Twist</t>
+  </si>
+  <si>
+    <t>Stoker, Bram</t>
+  </si>
+  <si>
+    <t>978-9066-0465-7399-3</t>
+  </si>
+  <si>
+    <t>Middlemarch</t>
+  </si>
+  <si>
+    <t>Twain, Mark</t>
+  </si>
+  <si>
+    <t>978-7880-7257-1288-0</t>
+  </si>
+  <si>
+    <t>The Scarlet Letter</t>
+  </si>
+  <si>
+    <t>Bronte, Emily</t>
+  </si>
+  <si>
+    <t>978-1542-2780-3031-9</t>
+  </si>
+  <si>
+    <t>Huxley, Aldous</t>
+  </si>
+  <si>
+    <t>978-1658-6920-5226-8</t>
+  </si>
+  <si>
+    <t>Austen, Jane</t>
+  </si>
+  <si>
+    <t>978-0128-9499-3068-1</t>
+  </si>
+  <si>
+    <t>Dickens, Charles</t>
+  </si>
+  <si>
+    <t>978-5537-6891-7648-0</t>
+  </si>
+  <si>
+    <t>War of the Worlds</t>
+  </si>
+  <si>
+    <t>Hawthorne, Nathaniel</t>
+  </si>
+  <si>
+    <t>978-5876-3791-6016-3</t>
+  </si>
+  <si>
+    <t>Melville, Herman</t>
+  </si>
+  <si>
+    <t>978-5933-2634-2907-4</t>
+  </si>
+  <si>
+    <t>The Iliad</t>
+  </si>
+  <si>
+    <t>Tolkien, J.R.R.</t>
+  </si>
+  <si>
+    <t>978-0321-7520-5196-9</t>
+  </si>
+  <si>
+    <t>Gulliver's Travels</t>
+  </si>
+  <si>
+    <t>Mann, Thomas</t>
+  </si>
+  <si>
+    <t>978-2076-9639-4647-6</t>
+  </si>
+  <si>
+    <t>Great Expectations</t>
+  </si>
+  <si>
+    <t>978-3643-0980-7638-0</t>
+  </si>
+  <si>
+    <t>Lolita</t>
+  </si>
+  <si>
+    <t>Kafka, Franz</t>
+  </si>
+  <si>
+    <t>978-1007-3439-2339-0</t>
+  </si>
+  <si>
+    <t>978-3385-8534-6423-9</t>
+  </si>
+  <si>
+    <t>To Kill a Mockingbird</t>
+  </si>
+  <si>
+    <t>Shelley, Mary</t>
+  </si>
+  <si>
+    <t>978-3021-8348-4386-4</t>
+  </si>
+  <si>
+    <t>Orwell, George</t>
+  </si>
+  <si>
+    <t>978-9204-2361-3358-5</t>
+  </si>
+  <si>
+    <t>The Divine Comedy</t>
+  </si>
+  <si>
+    <t>978-2859-0320-2167-5</t>
+  </si>
+  <si>
+    <t>978-0211-2527-2162-8</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings</t>
+  </si>
+  <si>
+    <t>Dostoevsky, Fyodor</t>
+  </si>
+  <si>
+    <t>978-8298-9758-7572-2</t>
+  </si>
+  <si>
+    <t>Madame Bovary</t>
+  </si>
+  <si>
+    <t>Dumas, Alexandre</t>
+  </si>
+  <si>
+    <t>978-1455-7910-8668-0</t>
   </si>
   <si>
     <t>Anna Karenina</t>
+  </si>
+  <si>
+    <t>978-9392-8278-3058-5</t>
+  </si>
+  <si>
+    <t>East of Eden</t>
+  </si>
+  <si>
+    <t>978-7131-0978-0904-3</t>
+  </si>
+  <si>
+    <t>Catch-22</t>
+  </si>
+  <si>
+    <t>978-6868-6228-3104-9</t>
+  </si>
+  <si>
+    <t>Don Quixote</t>
+  </si>
+  <si>
+    <t>978-3366-0465-6763-7</t>
+  </si>
+  <si>
+    <t>Carroll, Lewis</t>
+  </si>
+  <si>
+    <t>978-9236-2361-9584-1</t>
+  </si>
+  <si>
+    <t>978-2724-9605-2900-8</t>
+  </si>
+  <si>
+    <t>Dracula</t>
+  </si>
+  <si>
+    <t>978-9287-8425-7804-5</t>
+  </si>
+  <si>
+    <t>Pride and Prejudice</t>
+  </si>
+  <si>
+    <t>978-5517-2133-1659-8</t>
+  </si>
+  <si>
+    <t>Eliot, George</t>
+  </si>
+  <si>
+    <t>978-7930-2790-5138-8</t>
+  </si>
+  <si>
+    <t>978-0409-9077-7707-3</t>
+  </si>
+  <si>
+    <t>The Metamorphosis</t>
+  </si>
+  <si>
+    <t>978-9720-6126-6817-6</t>
+  </si>
+  <si>
+    <t>The Stranger</t>
+  </si>
+  <si>
+    <t>978-6440-2980-1796-8</t>
+  </si>
+  <si>
+    <t>Marquez, Gabriel Garcia</t>
+  </si>
+  <si>
+    <t>978-2662-1667-7068-8</t>
+  </si>
+  <si>
+    <t>Crime and Punishment</t>
+  </si>
+  <si>
+    <t>978-6497-9888-4009-7</t>
+  </si>
+  <si>
+    <t>The Great Gatsby</t>
+  </si>
+  <si>
+    <t>978-7130-1771-1583-7</t>
+  </si>
+  <si>
+    <t>Ulysses</t>
+  </si>
+  <si>
+    <t>978-3058-7923-2961-8</t>
+  </si>
+  <si>
+    <t>978-6418-1738-5828-3</t>
+  </si>
+  <si>
+    <t>978-9134-6414-1532-7</t>
   </si>
 </sst>
 </file>
@@ -289,21 +619,711 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2007.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1893.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2012.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1993.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1922.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1888.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2020.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1879.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2016.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1990.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1939.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1951.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1866.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2012.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1932.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2023.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1923.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1987.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1987.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2011.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1921.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1906.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2021.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1961.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1962.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1922.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1989.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1962.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1972.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>1984.0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1972.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1885.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1968.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2003.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1910.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1921.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1872.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1873.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1978.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1944.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1921.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1949.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>1984.0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1850.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1889.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1979.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1971.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1871.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1966.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1858.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1975.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1943.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>